<commit_message>
Update Editable labels, import format
- Able to import custom format in the designer
- You can update editable labels on imports (Fixed #259)
</commit_message>
<xml_diff>
--- a/misc/linelist_format.xlsx
+++ b/misc/linelist_format.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\outbreak-tools\misc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9FF0A-E7D9-4C3B-AFCE-555517974C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="24" windowWidth="29604" windowHeight="13776"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LinelistStyle" sheetId="1" r:id="rId1"/>
@@ -23,35 +29,8 @@
     <definedName name="TABLES_STYLES_LIST">LinelistStyle!$K$2:$K$63</definedName>
     <definedName name="UserLangList">[1]DesignerTranslation!$B$145:$B$149</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" iterate="1" iterateCount="1" calcCompleted="0" calcOnSave="0"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>tc={CC8C3746-92CC-471D-A9D3-2E0A1638A959}</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Insert your own design here the colors in the cell are used in the linelist</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,7 +417,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -550,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,6 +719,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1088,6 +1073,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1253,13 +1241,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="double">
-          <color theme="2" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="hair">
           <color auto="1"/>
         </left>
@@ -1271,6 +1252,13 @@
         </top>
         <bottom style="hair">
           <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="2" tint="-0.499984740745262"/>
         </bottom>
       </border>
     </dxf>
@@ -1308,13 +1296,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="__names"/>
       <sheetName val="Main"/>
@@ -1348,16 +1342,7 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="330">
-          <cell r="E330" t="str">
-            <v>English</v>
-          </cell>
-          <cell r="F330" t="str">
-            <v>ENG</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11">
         <row r="141">
           <cell r="C141" t="str">
@@ -1389,16 +1374,6 @@
             <v>Español</v>
           </cell>
         </row>
-        <row r="153">
-          <cell r="B153" t="str">
-            <v>English</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="B154" t="str">
-            <v>Français</v>
-          </cell>
-        </row>
       </sheetData>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
@@ -1408,26 +1383,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table26" displayName="Table26" ref="A1:E45" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6">
-  <autoFilter ref="A1:E45"/>
-  <sortState ref="A2:E45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table26" displayName="Table26" ref="A1:E45" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
     <sortCondition ref="B1:B45"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="scope" dataDxfId="4"/>
-    <tableColumn id="2" name="label" dataDxfId="3"/>
-    <tableColumn id="3" name="design 1" dataDxfId="2"/>
-    <tableColumn id="4" name="design 2" dataDxfId="1"/>
-    <tableColumn id="5" name="user defined" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="scope" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="label" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="design 1" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="design 2" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="user defined" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1465,7 +1440,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1537,7 +1512,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1710,13 +1685,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" customWidth="1"/>
@@ -1802,7 +1779,7 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="E3" s="72"/>
       <c r="J3">
         <v>2</v>
       </c>
@@ -3083,22 +3060,30 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32:E32">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 E18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 E18" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>TABLES_STYLES_LIST</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3A3FB3F943FF46B1D26EE220E8F380" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09af5b0cc4c0ce8c832fdadddb1f2960">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cf337b8-73be-4868-8a82-fc646b92f009" xmlns:ns3="126fb4af-9c28-4c50-9bd6-cb082ad1c16e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f16376d759aef0024467508612357766" ns2:_="" ns3:_="">
     <xsd:import namespace="8cf337b8-73be-4868-8a82-fc646b92f009"/>
@@ -3269,19 +3254,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D3B6BE2-0E31-40AB-8DDF-FB22B2D95D3B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC384962-C6E7-4070-A921-3C9E636DC61A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC384962-C6E7-4070-A921-3C9E636DC61A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D3B6BE2-0E31-40AB-8DDF-FB22B2D95D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8cf337b8-73be-4868-8a82-fc646b92f009"/>
+    <ds:schemaRef ds:uri="126fb4af-9c28-4c50-9bd6-cb082ad1c16e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>